<commit_message>
Marked Action Required tests for execution
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>TCID</t>
   </si>
@@ -88,6 +88,27 @@
   </si>
   <si>
     <t>Creates a new Transmittal of  Issue Reason  IssuedForApproval</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_ActionRequired_New_RequestForInformation</t>
+  </si>
+  <si>
+    <t>Creates a new Transmittal of  Issue Reason  IssuedForApproval and perform submission from Action Required Page</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_ActionRequired_New_IssuedForReview</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_ActionRequired_New_IssuedForApproval</t>
+  </si>
+  <si>
+    <t>Sprint2</t>
+  </si>
+  <si>
+    <t>Creates a new Transmittal of  Issue Reason  IssuedForReview and perform submission from Action Required Page</t>
+  </si>
+  <si>
+    <t>Creates a new Transmittal of  Issue Reason  RequestForInformation and perform submission from Action Required Page</t>
   </si>
 </sst>
 </file>
@@ -519,7 +540,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -678,12 +699,66 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30">
+      <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D11">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Marked FLD_Transmittals_ActionRequired_CaC_IssuedForReview for execution
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>TCID</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Creates a new Transmittal of  Issue Reason  RequestForInformation and perform submission from Action Required Page</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_ActionRequired_CaC_IssuedForReview</t>
+  </si>
+  <si>
+    <t>Verifies the Close and Cancel option for the user in the Transmital record</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -186,13 +195,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,9 +552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -753,17 +767,37 @@
         <v>27</v>
       </c>
     </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D12">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F12">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Marked for execution FLD_Transmittals_ActionRequired_CaC_RequestForInformation,FLD_Transmittals_ActionRequired_CaC_IssuedForApproval
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
   <si>
     <t>TCID</t>
   </si>
@@ -117,7 +117,13 @@
     <t>Verifies the Close and Cancel option for the user in the Transmital record</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>FLD_Transmittals_ActionRequired_CaC_RequestForInformation</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_ActionRequired_CaC_IssuedForApproval</t>
+  </si>
+  <si>
+    <t>Sprint3</t>
   </si>
 </sst>
 </file>
@@ -552,18 +558,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="49.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="73.28515625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -652,7 +656,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
@@ -670,7 +674,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
@@ -688,7 +692,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
@@ -706,7 +710,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
@@ -780,19 +784,53 @@
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30">
+      <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>27</v>
+      <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30">
+      <c r="A14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D14">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F14">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Marked tests for execution (till date developed)
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t>TCID</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Sprint3</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_LeftNavigationBar</t>
+  </si>
+  <si>
+    <t>Verifies the Left Navigation menu items</t>
   </si>
 </sst>
 </file>
@@ -558,9 +564,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -656,7 +664,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
@@ -674,7 +682,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
@@ -692,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
@@ -710,7 +718,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
@@ -825,12 +833,30 @@
         <v>34</v>
       </c>
     </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D15">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F15">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Included FLD_Transmittals_OverDue_New_IssuedForReview for execution.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS_Sprint5\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
   <si>
     <t>TCID</t>
   </si>
@@ -123,19 +123,25 @@
     <t>FLD_Transmittals_ActionRequired_CaC_IssuedForApproval</t>
   </si>
   <si>
-    <t>Sprint3</t>
-  </si>
-  <si>
     <t>FLD_Transmittals_LeftNavigationBar</t>
   </si>
   <si>
     <t>Verifies the Left Navigation menu items</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_OverDue_New_IssuedForReview</t>
+  </si>
+  <si>
+    <t>Verifies the transmittal under Actions Overdue menu</t>
+  </si>
+  <si>
+    <t>Sprint5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -207,7 +213,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -216,6 +222,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -564,7 +576,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -794,7 +806,7 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30">
@@ -812,7 +824,7 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30">
@@ -830,15 +842,15 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>7</v>
@@ -851,12 +863,30 @@
         <v>27</v>
       </c>
     </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D16">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F16">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>